<commit_message>
refactor and enrich code
</commit_message>
<xml_diff>
--- a/docs/Schema Design.xlsx
+++ b/docs/Schema Design.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\zProfessional_Projects\dev-workspace\mashreq-internal\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\zProfessional_Projects\dev-workspace\mashreq-internal\crbservice\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FBCDC5F-1146-43AA-87EB-714ECD323CC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{642F7447-57D2-4A49-A254-CBC24F698EB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{16BB6BC0-3788-41D3-B548-0B313D7C807A}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="51">
   <si>
     <t>id</t>
   </si>
@@ -120,15 +120,9 @@
     <t>working_hour_window</t>
   </si>
   <si>
-    <t>9:00 - 18:00</t>
-  </si>
-  <si>
     <t>maintenance_slot</t>
   </si>
   <si>
-    <t>9:00 - 9:15</t>
-  </si>
-  <si>
     <t>13:00 - 13:15</t>
   </si>
   <si>
@@ -150,15 +144,6 @@
     <t>2024-03-25</t>
   </si>
   <si>
-    <t>9:15 - 9:30</t>
-  </si>
-  <si>
-    <t>9:30 - 9:45</t>
-  </si>
-  <si>
-    <t>9:45 - 10:00</t>
-  </si>
-  <si>
     <t>10:00 - 10:15</t>
   </si>
   <si>
@@ -172,6 +157,27 @@
   </si>
   <si>
     <t>audit_fields</t>
+  </si>
+  <si>
+    <t>09:00 - 18:00</t>
+  </si>
+  <si>
+    <t>09:45 - 10:00</t>
+  </si>
+  <si>
+    <t>09:00 - 09:15</t>
+  </si>
+  <si>
+    <t>09:15 - 09:30</t>
+  </si>
+  <si>
+    <t>09:30 - 09:45</t>
+  </si>
+  <si>
+    <t>2,3,4</t>
+  </si>
+  <si>
+    <t>9</t>
   </si>
 </sst>
 </file>
@@ -272,24 +278,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" indent="2"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="left" indent="2"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1"/>
@@ -309,10 +310,10 @@
     <xf numFmtId="20" fontId="0" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="20" fontId="0" fillId="3" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" indent="2"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" indent="2"/>
     </xf>
     <xf numFmtId="20" fontId="0" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -329,6 +330,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -644,15 +648,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F127CAD6-A88D-48D0-BF65-9CE8D305B654}">
-  <dimension ref="B1:U46"/>
+  <dimension ref="B1:T46"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="H23" sqref="H23"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="M37" sqref="M37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="4.453125" customWidth="1"/>
+    <col min="1" max="1" width="1.90625" customWidth="1"/>
     <col min="3" max="3" width="18.81640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="19.1796875" customWidth="1"/>
     <col min="5" max="5" width="17" customWidth="1"/>
@@ -672,44 +676,44 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:15" x14ac:dyDescent="0.35">
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="24" t="s">
         <v>21</v>
       </c>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
-      <c r="J1" s="5"/>
-      <c r="K1" s="5"/>
-      <c r="L1" s="5"/>
-      <c r="M1" s="5"/>
-      <c r="N1" s="5"/>
-      <c r="O1" s="5"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
+      <c r="I1" s="24"/>
+      <c r="J1" s="24"/>
+      <c r="K1" s="24"/>
+      <c r="L1" s="24"/>
+      <c r="M1" s="24"/>
+      <c r="N1" s="24"/>
+      <c r="O1" s="24"/>
     </row>
     <row r="2" spans="2:15" x14ac:dyDescent="0.35">
-      <c r="B2" s="5"/>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
-      <c r="H2" s="5"/>
-      <c r="I2" s="5"/>
-      <c r="J2" s="5"/>
-      <c r="K2" s="5"/>
-      <c r="L2" s="5"/>
-      <c r="M2" s="5"/>
-      <c r="N2" s="5"/>
-      <c r="O2" s="5"/>
+      <c r="B2" s="24"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
+      <c r="F2" s="24"/>
+      <c r="G2" s="24"/>
+      <c r="H2" s="24"/>
+      <c r="I2" s="24"/>
+      <c r="J2" s="24"/>
+      <c r="K2" s="24"/>
+      <c r="L2" s="24"/>
+      <c r="M2" s="24"/>
+      <c r="N2" s="24"/>
+      <c r="O2" s="24"/>
     </row>
     <row r="3" spans="2:15" x14ac:dyDescent="0.35">
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="K3" s="4" t="s">
+      <c r="K3" s="3" t="s">
         <v>27</v>
       </c>
     </row>
@@ -733,7 +737,7 @@
         <v>30</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="K4" s="1" t="s">
         <v>0</v>
@@ -741,13 +745,12 @@
       <c r="L4" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="M4" s="15" t="s">
-        <v>32</v>
+      <c r="M4" s="12" t="s">
+        <v>31</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="O4" s="2"/>
+        <v>43</v>
+      </c>
     </row>
     <row r="5" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B5" s="1">
@@ -765,21 +768,20 @@
       <c r="F5" s="1">
         <v>15</v>
       </c>
-      <c r="G5" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="H5" s="12"/>
+      <c r="G5" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="H5" s="9"/>
       <c r="K5" s="1">
         <v>1</v>
       </c>
       <c r="L5" s="1">
         <v>1</v>
       </c>
-      <c r="M5" s="14" t="s">
-        <v>33</v>
-      </c>
-      <c r="N5" s="3"/>
-      <c r="O5" s="2"/>
+      <c r="M5" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="N5" s="2"/>
     </row>
     <row r="6" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B6" s="1">
@@ -797,21 +799,20 @@
       <c r="F6" s="1">
         <v>15</v>
       </c>
-      <c r="G6" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="H6" s="12"/>
+      <c r="G6" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="H6" s="9"/>
       <c r="K6" s="1">
         <v>2</v>
       </c>
       <c r="L6" s="1">
         <v>1</v>
       </c>
-      <c r="M6" s="14" t="s">
-        <v>34</v>
-      </c>
-      <c r="N6" s="3"/>
-      <c r="O6" s="2"/>
+      <c r="M6" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="N6" s="2"/>
     </row>
     <row r="7" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B7" s="1">
@@ -829,21 +830,20 @@
       <c r="F7" s="1">
         <v>15</v>
       </c>
-      <c r="G7" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="H7" s="12"/>
+      <c r="G7" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="H7" s="9"/>
       <c r="K7" s="1">
         <v>3</v>
       </c>
       <c r="L7" s="1">
         <v>1</v>
       </c>
-      <c r="M7" s="14" t="s">
-        <v>35</v>
-      </c>
-      <c r="N7" s="3"/>
-      <c r="O7" s="2"/>
+      <c r="M7" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="N7" s="2"/>
     </row>
     <row r="8" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B8" s="1">
@@ -861,21 +861,20 @@
       <c r="F8" s="1">
         <v>15</v>
       </c>
-      <c r="G8" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="H8" s="12"/>
+      <c r="G8" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="H8" s="9"/>
       <c r="K8" s="1">
         <v>4</v>
       </c>
       <c r="L8" s="1">
         <v>2</v>
       </c>
-      <c r="M8" s="14" t="s">
-        <v>33</v>
-      </c>
-      <c r="N8" s="3"/>
-      <c r="O8" s="2"/>
+      <c r="M8" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="N8" s="2"/>
     </row>
     <row r="9" spans="2:15" x14ac:dyDescent="0.35">
       <c r="K9" s="1">
@@ -884,11 +883,10 @@
       <c r="L9" s="1">
         <v>2</v>
       </c>
-      <c r="M9" s="14" t="s">
-        <v>34</v>
-      </c>
-      <c r="N9" s="3"/>
-      <c r="O9" s="2"/>
+      <c r="M9" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="N9" s="2"/>
     </row>
     <row r="10" spans="2:15" x14ac:dyDescent="0.35">
       <c r="K10" s="1">
@@ -897,11 +895,10 @@
       <c r="L10" s="1">
         <v>2</v>
       </c>
-      <c r="M10" s="14" t="s">
-        <v>35</v>
-      </c>
-      <c r="N10" s="3"/>
-      <c r="O10" s="2"/>
+      <c r="M10" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="N10" s="2"/>
     </row>
     <row r="11" spans="2:15" x14ac:dyDescent="0.35">
       <c r="K11" s="1">
@@ -910,11 +907,10 @@
       <c r="L11" s="1">
         <v>3</v>
       </c>
-      <c r="M11" s="14" t="s">
-        <v>33</v>
-      </c>
-      <c r="N11" s="3"/>
-      <c r="O11" s="2"/>
+      <c r="M11" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="N11" s="2"/>
     </row>
     <row r="12" spans="2:15" x14ac:dyDescent="0.35">
       <c r="K12" s="1">
@@ -923,31 +919,29 @@
       <c r="L12" s="1">
         <v>3</v>
       </c>
-      <c r="M12" s="14" t="s">
-        <v>34</v>
-      </c>
-      <c r="N12" s="3"/>
-      <c r="O12" s="2"/>
+      <c r="M12" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="N12" s="2"/>
     </row>
     <row r="13" spans="2:15" x14ac:dyDescent="0.35">
-      <c r="B13" s="4" t="s">
+      <c r="B13" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="G13" s="8" t="s">
+      <c r="G13" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="H13" s="8"/>
+      <c r="H13" s="5"/>
       <c r="K13" s="1">
         <v>9</v>
       </c>
       <c r="L13" s="1">
         <v>3</v>
       </c>
-      <c r="M13" s="14" t="s">
-        <v>35</v>
-      </c>
-      <c r="N13" s="3"/>
-      <c r="O13" s="2"/>
+      <c r="M13" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="N13" s="2"/>
     </row>
     <row r="14" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B14" s="1" t="s">
@@ -957,65 +951,59 @@
         <v>26</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F14" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="G14" s="21" t="s">
-        <v>37</v>
-      </c>
-      <c r="H14" s="21"/>
-      <c r="I14" s="2"/>
-      <c r="J14" s="2"/>
+      <c r="G14" s="18" t="s">
+        <v>35</v>
+      </c>
+      <c r="H14" s="18"/>
       <c r="K14" s="1">
         <v>10</v>
       </c>
       <c r="L14" s="1">
         <v>4</v>
       </c>
-      <c r="M14" s="14" t="s">
-        <v>33</v>
-      </c>
-      <c r="N14" s="3"/>
-      <c r="O14" s="2"/>
+      <c r="M14" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="N14" s="2"/>
     </row>
     <row r="15" spans="2:15" x14ac:dyDescent="0.35">
-      <c r="B15" s="16">
+      <c r="B15" s="13">
         <v>1</v>
       </c>
-      <c r="C15" s="16">
-        <v>2</v>
-      </c>
-      <c r="D15" s="17" t="s">
-        <v>40</v>
-      </c>
-      <c r="E15" s="22" t="s">
-        <v>33</v>
-      </c>
-      <c r="F15" s="16">
+      <c r="C15" s="13">
+        <v>2</v>
+      </c>
+      <c r="D15" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="E15" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="F15" s="13">
         <v>-1</v>
       </c>
-      <c r="G15" s="9" t="s">
+      <c r="G15" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="H15" s="9"/>
-      <c r="I15" s="2"/>
-      <c r="J15" s="2"/>
+      <c r="H15" s="6"/>
       <c r="K15" s="1">
         <v>11</v>
       </c>
       <c r="L15" s="1">
         <v>4</v>
       </c>
-      <c r="M15" s="14" t="s">
-        <v>34</v>
-      </c>
-      <c r="N15" s="3"/>
-      <c r="O15" s="2"/>
+      <c r="M15" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="N15" s="2"/>
     </row>
     <row r="16" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B16" s="1">
@@ -1024,157 +1012,117 @@
       <c r="C16" s="1">
         <v>2</v>
       </c>
-      <c r="D16" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="E16" s="14" t="s">
-        <v>41</v>
+      <c r="D16" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="E16" s="11" t="s">
+        <v>47</v>
       </c>
       <c r="F16" s="1">
         <v>0</v>
       </c>
-      <c r="G16" s="20" t="s">
+      <c r="G16" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="H16" s="20"/>
-      <c r="I16" s="2"/>
-      <c r="J16" s="2"/>
+      <c r="H16" s="17"/>
       <c r="K16" s="1">
         <v>12</v>
       </c>
       <c r="L16" s="1">
         <v>4</v>
       </c>
-      <c r="M16" s="14" t="s">
-        <v>35</v>
-      </c>
-      <c r="N16" s="3"/>
-      <c r="O16" s="2"/>
-    </row>
-    <row r="17" spans="2:21" x14ac:dyDescent="0.35">
-      <c r="B17" s="18">
+      <c r="M16" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="N16" s="2"/>
+    </row>
+    <row r="17" spans="2:20" x14ac:dyDescent="0.35">
+      <c r="B17" s="15">
         <v>3</v>
       </c>
-      <c r="C17" s="18">
-        <v>2</v>
-      </c>
-      <c r="D17" s="19" t="s">
-        <v>40</v>
-      </c>
-      <c r="E17" s="23" t="s">
-        <v>42</v>
-      </c>
-      <c r="F17" s="18">
+      <c r="C17" s="15">
+        <v>2</v>
+      </c>
+      <c r="D17" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="E17" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="F17" s="15">
         <v>1</v>
       </c>
-      <c r="G17" s="10"/>
-      <c r="H17" s="10"/>
-      <c r="I17" s="2"/>
-      <c r="J17" s="2"/>
-      <c r="K17" s="2"/>
-      <c r="L17" s="2"/>
-      <c r="M17" s="2"/>
-      <c r="N17" s="2"/>
-      <c r="O17" s="2"/>
-    </row>
-    <row r="18" spans="2:21" x14ac:dyDescent="0.35">
-      <c r="B18" s="18">
+      <c r="G17" s="7"/>
+      <c r="H17" s="7"/>
+    </row>
+    <row r="18" spans="2:20" x14ac:dyDescent="0.35">
+      <c r="B18" s="15">
         <v>4</v>
       </c>
-      <c r="C18" s="18">
-        <v>2</v>
-      </c>
-      <c r="D18" s="19" t="s">
-        <v>40</v>
-      </c>
-      <c r="E18" s="23" t="s">
-        <v>43</v>
-      </c>
-      <c r="F18" s="18">
+      <c r="C18" s="15">
+        <v>2</v>
+      </c>
+      <c r="D18" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="E18" s="20" t="s">
+        <v>45</v>
+      </c>
+      <c r="F18" s="15">
         <v>1</v>
       </c>
-      <c r="G18" s="2"/>
-      <c r="H18" s="2"/>
-      <c r="I18" s="2"/>
-      <c r="J18" s="2"/>
-      <c r="K18" s="2"/>
-      <c r="L18" s="2"/>
-      <c r="M18" s="2"/>
-      <c r="N18" s="2"/>
-      <c r="O18" s="2"/>
-    </row>
-    <row r="19" spans="2:21" x14ac:dyDescent="0.35">
+    </row>
+    <row r="19" spans="2:20" x14ac:dyDescent="0.35">
       <c r="B19" s="1">
         <v>5</v>
       </c>
       <c r="C19" s="1">
         <v>2</v>
       </c>
-      <c r="D19" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="E19" s="24" t="s">
-        <v>44</v>
+      <c r="D19" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="E19" s="21" t="s">
+        <v>39</v>
       </c>
       <c r="F19" s="1">
         <v>0</v>
       </c>
-      <c r="G19" s="2"/>
-      <c r="H19" s="2"/>
-      <c r="I19" s="2"/>
-      <c r="J19" s="2"/>
-      <c r="K19" s="2"/>
-      <c r="L19" s="2"/>
-      <c r="M19" s="2"/>
-      <c r="N19" s="2"/>
-      <c r="O19" s="2"/>
-    </row>
-    <row r="20" spans="2:21" x14ac:dyDescent="0.35">
+    </row>
+    <row r="20" spans="2:20" x14ac:dyDescent="0.35">
       <c r="B20" s="1">
         <v>6</v>
       </c>
       <c r="C20" s="1">
         <v>2</v>
       </c>
-      <c r="D20" s="11" t="s">
+      <c r="D20" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="E20" s="21" t="s">
         <v>40</v>
       </c>
-      <c r="E20" s="24" t="s">
-        <v>45</v>
-      </c>
       <c r="F20" s="1">
         <v>0</v>
       </c>
-      <c r="G20" s="2"/>
-      <c r="H20" s="2"/>
-      <c r="I20" s="2"/>
-      <c r="J20" s="2"/>
-      <c r="K20" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="L20" s="2"/>
-      <c r="M20" s="2"/>
-      <c r="N20" s="2"/>
-      <c r="O20" s="2"/>
-    </row>
-    <row r="21" spans="2:21" x14ac:dyDescent="0.35">
+      <c r="K20" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="21" spans="2:20" x14ac:dyDescent="0.35">
       <c r="B21" s="1">
         <v>7</v>
       </c>
       <c r="C21" s="1">
         <v>2</v>
       </c>
-      <c r="D21" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="E21" s="13"/>
+      <c r="D21" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="E21" s="10"/>
       <c r="F21" s="1">
         <v>0</v>
       </c>
-      <c r="G21" s="2"/>
-      <c r="H21" s="2"/>
-      <c r="I21" s="2"/>
-      <c r="J21" s="2"/>
       <c r="K21" s="1" t="s">
         <v>0</v>
       </c>
@@ -1203,118 +1151,114 @@
         <v>14</v>
       </c>
       <c r="T21" s="1" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="22" spans="2:21" x14ac:dyDescent="0.35">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="22" spans="2:20" x14ac:dyDescent="0.35">
       <c r="B22" s="1">
         <v>8</v>
       </c>
       <c r="C22" s="1">
         <v>2</v>
       </c>
-      <c r="D22" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="E22" s="13"/>
+      <c r="D22" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="E22" s="10"/>
       <c r="F22" s="1">
         <v>0</v>
       </c>
-      <c r="G22" s="2"/>
-      <c r="H22" s="2"/>
-      <c r="I22" s="2"/>
-      <c r="J22" s="2"/>
-      <c r="K22" s="13">
+      <c r="K22" s="10">
         <v>1</v>
       </c>
-      <c r="L22" s="13">
+      <c r="L22" s="10">
         <v>2</v>
       </c>
       <c r="M22" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="N22" s="7" t="s">
+      <c r="N22" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="O22" s="7" t="s">
+      <c r="O22" s="4" t="s">
         <v>17</v>
       </c>
       <c r="P22" s="1">
         <v>7</v>
       </c>
-      <c r="Q22" s="3">
+      <c r="Q22" s="2">
         <v>0.38541666666666669</v>
       </c>
-      <c r="R22" s="3">
+      <c r="R22" s="2">
         <v>0.41666666666666669</v>
       </c>
-      <c r="S22" s="1"/>
+      <c r="S22" s="4" t="s">
+        <v>49</v>
+      </c>
       <c r="T22" s="1"/>
     </row>
-    <row r="23" spans="2:21" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:20" x14ac:dyDescent="0.35">
       <c r="B23" s="1">
         <v>9</v>
       </c>
       <c r="C23" s="1">
         <v>2</v>
       </c>
-      <c r="D23" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="E23" s="13"/>
+      <c r="D23" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="E23" s="10"/>
       <c r="F23" s="1">
         <v>0</v>
       </c>
-      <c r="G23" s="2"/>
-      <c r="H23" s="2"/>
-      <c r="I23" s="2"/>
-      <c r="J23" s="2"/>
-      <c r="K23" s="13">
-        <v>2</v>
-      </c>
-      <c r="L23" s="13">
+      <c r="K23" s="10">
+        <v>2</v>
+      </c>
+      <c r="L23" s="10">
         <v>3</v>
       </c>
       <c r="M23" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="N23" s="7" t="s">
+      <c r="N23" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="O23" s="7" t="s">
+      <c r="O23" s="4" t="s">
         <v>20</v>
       </c>
       <c r="P23" s="1">
         <v>10</v>
       </c>
-      <c r="Q23" s="1"/>
-      <c r="R23" s="1"/>
-      <c r="S23" s="1"/>
+      <c r="Q23" s="2">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="R23" s="2">
+        <v>0.46875</v>
+      </c>
+      <c r="S23" s="4" t="s">
+        <v>50</v>
+      </c>
       <c r="T23" s="1"/>
     </row>
-    <row r="24" spans="2:21" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:20" x14ac:dyDescent="0.35">
       <c r="B24" s="1">
         <v>10</v>
       </c>
       <c r="C24" s="1">
         <v>2</v>
       </c>
-      <c r="D24" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="E24" s="13"/>
+      <c r="D24" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="E24" s="10"/>
       <c r="F24" s="1">
         <v>0</v>
       </c>
-      <c r="G24" s="2"/>
-      <c r="H24" s="2"/>
-      <c r="I24" s="2"/>
-      <c r="J24" s="2"/>
-      <c r="K24" s="13">
+      <c r="K24" s="10">
         <v>3</v>
       </c>
-      <c r="L24" s="13" t="s">
-        <v>36</v>
+      <c r="L24" s="10" t="s">
+        <v>34</v>
       </c>
       <c r="M24" s="1"/>
       <c r="N24" s="1"/>
@@ -1325,31 +1269,27 @@
       <c r="S24" s="1"/>
       <c r="T24" s="1"/>
     </row>
-    <row r="25" spans="2:21" x14ac:dyDescent="0.35">
-      <c r="B25" s="16">
+    <row r="25" spans="2:20" x14ac:dyDescent="0.35">
+      <c r="B25" s="13">
         <v>11</v>
       </c>
-      <c r="C25" s="16">
-        <v>2</v>
-      </c>
-      <c r="D25" s="17" t="s">
-        <v>40</v>
-      </c>
-      <c r="E25" s="25" t="s">
-        <v>46</v>
-      </c>
-      <c r="F25" s="16">
+      <c r="C25" s="13">
+        <v>2</v>
+      </c>
+      <c r="D25" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="E25" s="22" t="s">
+        <v>41</v>
+      </c>
+      <c r="F25" s="13">
         <v>-1</v>
       </c>
-      <c r="G25" s="2"/>
-      <c r="H25" s="2"/>
-      <c r="I25" s="2"/>
-      <c r="J25" s="2"/>
-      <c r="K25" s="13" t="s">
-        <v>36</v>
-      </c>
-      <c r="L25" s="13" t="s">
-        <v>36</v>
+      <c r="K25" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="L25" s="10" t="s">
+        <v>34</v>
       </c>
       <c r="M25" s="1"/>
       <c r="N25" s="1"/>
@@ -1360,27 +1300,25 @@
       <c r="S25" s="1"/>
       <c r="T25" s="1"/>
     </row>
-    <row r="26" spans="2:21" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:20" x14ac:dyDescent="0.35">
       <c r="B26" s="1">
         <v>12</v>
       </c>
       <c r="C26" s="1">
         <v>2</v>
       </c>
-      <c r="D26" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="E26" s="13"/>
+      <c r="D26" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="E26" s="10"/>
       <c r="F26" s="1">
         <v>0</v>
       </c>
-      <c r="G26" s="2"/>
-      <c r="H26" s="2"/>
-      <c r="K26" s="13" t="s">
-        <v>36</v>
-      </c>
-      <c r="L26" s="13" t="s">
-        <v>36</v>
+      <c r="K26" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="L26" s="10" t="s">
+        <v>34</v>
       </c>
       <c r="M26" s="1"/>
       <c r="N26" s="1"/>
@@ -1391,126 +1329,94 @@
       <c r="S26" s="1"/>
       <c r="T26" s="1"/>
     </row>
-    <row r="27" spans="2:21" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:20" x14ac:dyDescent="0.35">
       <c r="B27" s="1">
         <v>13</v>
       </c>
       <c r="C27" s="1">
         <v>2</v>
       </c>
-      <c r="D27" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="E27" s="13"/>
+      <c r="D27" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="E27" s="10"/>
       <c r="F27" s="1">
         <v>0</v>
       </c>
-      <c r="G27" s="2"/>
-      <c r="H27" s="2"/>
-      <c r="K27" s="2"/>
-      <c r="L27" s="2"/>
-      <c r="M27" s="2"/>
-      <c r="N27" s="2"/>
-      <c r="O27" s="2"/>
-      <c r="P27" s="2"/>
-      <c r="Q27" s="2"/>
-      <c r="R27" s="2"/>
-      <c r="S27" s="2"/>
-      <c r="T27" s="2"/>
-      <c r="U27" s="2"/>
-    </row>
-    <row r="28" spans="2:21" x14ac:dyDescent="0.35">
+    </row>
+    <row r="28" spans="2:20" x14ac:dyDescent="0.35">
       <c r="B28" s="1">
         <v>14</v>
       </c>
       <c r="C28" s="1">
         <v>2</v>
       </c>
-      <c r="D28" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="E28" s="13"/>
+      <c r="D28" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="E28" s="10"/>
       <c r="F28" s="1">
         <v>0</v>
       </c>
-      <c r="G28" s="2"/>
-      <c r="H28" s="2"/>
-      <c r="K28" s="2"/>
-      <c r="L28" s="2"/>
-      <c r="M28" s="2"/>
-      <c r="N28" s="2"/>
-      <c r="O28" s="2"/>
-      <c r="P28" s="2"/>
-      <c r="Q28" s="2"/>
-      <c r="R28" s="2"/>
-      <c r="S28" s="2"/>
-      <c r="T28" s="2"/>
-      <c r="U28" s="2"/>
-    </row>
-    <row r="29" spans="2:21" x14ac:dyDescent="0.35">
+    </row>
+    <row r="29" spans="2:20" x14ac:dyDescent="0.35">
       <c r="B29" s="1">
         <v>15</v>
       </c>
       <c r="C29" s="1">
         <v>2</v>
       </c>
-      <c r="D29" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="E29" s="13"/>
+      <c r="D29" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="E29" s="10"/>
       <c r="F29" s="1">
         <v>0</v>
       </c>
-      <c r="G29" s="2"/>
-      <c r="H29" s="2"/>
-    </row>
-    <row r="30" spans="2:21" x14ac:dyDescent="0.35">
+    </row>
+    <row r="30" spans="2:20" x14ac:dyDescent="0.35">
       <c r="B30" s="1">
         <v>16</v>
       </c>
       <c r="C30" s="1">
         <v>2</v>
       </c>
-      <c r="D30" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="E30" s="13"/>
+      <c r="D30" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="E30" s="10"/>
       <c r="F30" s="1">
         <v>0</v>
       </c>
-      <c r="G30" s="2"/>
-      <c r="H30" s="2"/>
-    </row>
-    <row r="31" spans="2:21" x14ac:dyDescent="0.35">
-      <c r="B31" s="16">
+    </row>
+    <row r="31" spans="2:20" x14ac:dyDescent="0.35">
+      <c r="B31" s="13">
         <v>17</v>
       </c>
-      <c r="C31" s="16">
-        <v>2</v>
-      </c>
-      <c r="D31" s="17" t="s">
-        <v>40</v>
-      </c>
-      <c r="E31" s="26" t="s">
-        <v>35</v>
-      </c>
-      <c r="F31" s="16">
+      <c r="C31" s="13">
+        <v>2</v>
+      </c>
+      <c r="D31" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="E31" s="23" t="s">
+        <v>33</v>
+      </c>
+      <c r="F31" s="13">
         <v>-1</v>
       </c>
-      <c r="G31" s="2"/>
-      <c r="H31" s="2"/>
-    </row>
-    <row r="32" spans="2:21" x14ac:dyDescent="0.35">
+    </row>
+    <row r="32" spans="2:20" x14ac:dyDescent="0.35">
       <c r="B32" s="1">
         <v>18</v>
       </c>
       <c r="C32" s="1">
         <v>2</v>
       </c>
-      <c r="D32" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="E32" s="13"/>
+      <c r="D32" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="E32" s="10"/>
       <c r="F32" s="1">
         <v>0</v>
       </c>
@@ -1522,10 +1428,10 @@
       <c r="C33" s="1">
         <v>2</v>
       </c>
-      <c r="D33" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="E33" s="13"/>
+      <c r="D33" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="E33" s="10"/>
       <c r="F33" s="1">
         <v>0</v>
       </c>
@@ -1537,10 +1443,10 @@
       <c r="C34" s="1">
         <v>2</v>
       </c>
-      <c r="D34" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="E34" s="13"/>
+      <c r="D34" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="E34" s="10"/>
       <c r="F34" s="1">
         <v>0</v>
       </c>
@@ -1552,10 +1458,10 @@
       <c r="C35" s="1">
         <v>2</v>
       </c>
-      <c r="D35" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="E35" s="13"/>
+      <c r="D35" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="E35" s="10"/>
       <c r="F35" s="1">
         <v>0</v>
       </c>
@@ -1567,8 +1473,8 @@
       <c r="C36" s="1">
         <v>2</v>
       </c>
-      <c r="D36" s="11" t="s">
-        <v>40</v>
+      <c r="D36" s="8" t="s">
+        <v>38</v>
       </c>
       <c r="E36" s="1"/>
       <c r="F36" s="1">
@@ -1582,8 +1488,8 @@
       <c r="C37" s="1">
         <v>2</v>
       </c>
-      <c r="D37" s="11" t="s">
-        <v>40</v>
+      <c r="D37" s="8" t="s">
+        <v>38</v>
       </c>
       <c r="E37" s="1"/>
       <c r="F37" s="1">
@@ -1597,8 +1503,8 @@
       <c r="C38" s="1">
         <v>2</v>
       </c>
-      <c r="D38" s="11" t="s">
-        <v>40</v>
+      <c r="D38" s="8" t="s">
+        <v>38</v>
       </c>
       <c r="E38" s="1"/>
       <c r="F38" s="1">
@@ -1612,8 +1518,8 @@
       <c r="C39" s="1">
         <v>2</v>
       </c>
-      <c r="D39" s="11" t="s">
-        <v>40</v>
+      <c r="D39" s="8" t="s">
+        <v>38</v>
       </c>
       <c r="E39" s="1"/>
       <c r="F39" s="1">
@@ -1627,8 +1533,8 @@
       <c r="C40" s="1">
         <v>2</v>
       </c>
-      <c r="D40" s="11" t="s">
-        <v>40</v>
+      <c r="D40" s="8" t="s">
+        <v>38</v>
       </c>
       <c r="E40" s="1"/>
       <c r="F40" s="1">
@@ -1642,8 +1548,8 @@
       <c r="C41" s="1">
         <v>2</v>
       </c>
-      <c r="D41" s="11" t="s">
-        <v>40</v>
+      <c r="D41" s="8" t="s">
+        <v>38</v>
       </c>
       <c r="E41" s="1"/>
       <c r="F41" s="1">
@@ -1657,8 +1563,8 @@
       <c r="C42" s="1">
         <v>2</v>
       </c>
-      <c r="D42" s="11" t="s">
-        <v>40</v>
+      <c r="D42" s="8" t="s">
+        <v>38</v>
       </c>
       <c r="E42" s="1"/>
       <c r="F42" s="1">
@@ -1672,8 +1578,8 @@
       <c r="C43" s="1">
         <v>2</v>
       </c>
-      <c r="D43" s="11" t="s">
-        <v>40</v>
+      <c r="D43" s="8" t="s">
+        <v>38</v>
       </c>
       <c r="E43" s="1"/>
       <c r="F43" s="1">
@@ -1687,8 +1593,8 @@
       <c r="C44" s="1">
         <v>2</v>
       </c>
-      <c r="D44" s="11" t="s">
-        <v>40</v>
+      <c r="D44" s="8" t="s">
+        <v>38</v>
       </c>
       <c r="E44" s="1"/>
       <c r="F44" s="1">
@@ -1702,8 +1608,8 @@
       <c r="C45" s="1">
         <v>2</v>
       </c>
-      <c r="D45" s="11" t="s">
-        <v>40</v>
+      <c r="D45" s="8" t="s">
+        <v>38</v>
       </c>
       <c r="E45" s="1"/>
       <c r="F45" s="1">
@@ -1717,8 +1623,8 @@
       <c r="C46" s="1">
         <v>2</v>
       </c>
-      <c r="D46" s="11" t="s">
-        <v>40</v>
+      <c r="D46" s="8" t="s">
+        <v>38</v>
       </c>
       <c r="E46" s="1"/>
       <c r="F46" s="1">

</xml_diff>

<commit_message>
code enrich and add validation in create booking
</commit_message>
<xml_diff>
--- a/docs/Schema Design.xlsx
+++ b/docs/Schema Design.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\zProfessional_Projects\dev-workspace\mashreq-internal\crbservice\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{642F7447-57D2-4A49-A254-CBC24F698EB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52AA2F3A-4649-4D41-AC14-BC697E251676}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{16BB6BC0-3788-41D3-B548-0B313D7C807A}"/>
   </bookViews>
@@ -651,16 +651,17 @@
   <dimension ref="B1:T46"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="M37" sqref="M37"/>
+      <selection activeCell="P41" sqref="P41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="1.90625" customWidth="1"/>
+    <col min="2" max="2" width="6.90625" customWidth="1"/>
     <col min="3" max="3" width="18.81640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.1796875" customWidth="1"/>
-    <col min="5" max="5" width="17" customWidth="1"/>
-    <col min="6" max="6" width="19.7265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.90625" customWidth="1"/>
+    <col min="5" max="5" width="16.36328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.81640625" customWidth="1"/>
     <col min="7" max="7" width="20.26953125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="6.36328125" customWidth="1"/>

</xml_diff>

<commit_message>
clean and update readme file
</commit_message>
<xml_diff>
--- a/docs/Schema Design.xlsx
+++ b/docs/Schema Design.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\zProfessional_Projects\dev-workspace\mashreq-internal\crbservice\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC44A1D2-35F9-4FCC-AB87-31F92C923F13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C347B3A-6C38-4498-B1DC-53C738167086}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{16BB6BC0-3788-41D3-B548-0B313D7C807A}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{16BB6BC0-3788-41D3-B548-0B313D7C807A}"/>
   </bookViews>
   <sheets>
     <sheet name="Schema Design" sheetId="1" r:id="rId1"/>
@@ -650,16 +650,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F127CAD6-A88D-48D0-BF65-9CE8D305B654}">
   <dimension ref="B1:T46"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="D1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="I20" sqref="I20"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
+      <selection activeCell="N40" sqref="N40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="1.90625" customWidth="1"/>
     <col min="2" max="2" width="6.90625" customWidth="1"/>
-    <col min="3" max="3" width="18.81640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.90625" customWidth="1"/>
+    <col min="3" max="3" width="18.54296875" customWidth="1"/>
+    <col min="4" max="4" width="18.36328125" customWidth="1"/>
     <col min="5" max="5" width="16.36328125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="19.81640625" customWidth="1"/>
     <col min="7" max="7" width="20.26953125" bestFit="1" customWidth="1"/>

</xml_diff>